<commit_message>
added Acer DRC genofit per timepoint
</commit_message>
<xml_diff>
--- a/ED50/Past_Offshore_Genets_ED50.xlsx
+++ b/ED50/Past_Offshore_Genets_ED50.xlsx
@@ -392,7 +392,7 @@
         <v>36.31368496448474</v>
       </c>
       <c r="D2">
-        <v>36.79823847929714</v>
+        <v>36.7982384792938</v>
       </c>
     </row>
     <row r="3">
@@ -408,7 +408,7 @@
         <v>37.13241740625019</v>
       </c>
       <c r="D3">
-        <v>37.51616355034255</v>
+        <v>37.51616355034346</v>
       </c>
     </row>
     <row r="4">
@@ -424,7 +424,7 @@
         <v>36.49173363241678</v>
       </c>
       <c r="D4">
-        <v>37.09873261463982</v>
+        <v>37.09873261463852</v>
       </c>
     </row>
     <row r="5">
@@ -440,7 +440,7 @@
         <v>37.30539930924083</v>
       </c>
       <c r="D5">
-        <v>37.12158476725192</v>
+        <v>37.12158476725313</v>
       </c>
     </row>
     <row r="6">
@@ -456,7 +456,7 @@
         <v>37.50078343496988</v>
       </c>
       <c r="D6">
-        <v>37.18812364602521</v>
+        <v>37.18812364602488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>